<commit_message>
Progress on Java 24 article
</commit_message>
<xml_diff>
--- a/_drafts/jep-overview.xlsx
+++ b/_drafts/jep-overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanno/Code/websites/hanno.codes/_drafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4CF600-EEFD-934D-9D75-DC3D5836F08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68EC1E7-89C4-E949-ADDC-A331C209AB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{D428FD44-A7BE-744F-BBBE-F876344939DC}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{D428FD44-A7BE-744F-BBBE-F876344939DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$25</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -596,7 +596,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,7 +722,7 @@
         <v>### JEP 475: Late Barrier Expansion for G1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>478</v>
       </c>
@@ -788,7 +788,7 @@
         <v>### JEP 483: Ahead-of-Time Class Loading &amp; Linking</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>484</v>
       </c>
@@ -809,7 +809,7 @@
         <v>### JEP 484: Class-File API</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>485</v>
       </c>
@@ -830,7 +830,7 @@
         <v>### JEP 485: Stream Gatherers</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>486</v>
       </c>
@@ -851,7 +851,7 @@
         <v>### JEP 486: Permanently Disable the Security Manager</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>487</v>
       </c>
@@ -875,7 +875,7 @@
         <v>### JEP 487: Scoped Values (Fourth Preview)</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>488</v>
       </c>
@@ -899,7 +899,7 @@
         <v>### JEP 488: Primitive Types in Patterns, instanceof and switch (Second Preview)</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>489</v>
       </c>
@@ -965,7 +965,7 @@
         <v>### JEP 491: Synchronize Virtual Threads Without Pinning</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>492</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>### JEP 493: Linking Run-Time Images Without JMODs</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>494</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>### JEP 494: Module Import Declarations (Second Preview)</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>495</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>### JEP 495: Simple Source Files and Instance Main Methods (Fourth Preview)</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>496</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>### JEP 496: Quantum-Resistant Module-Lattice-Based Key Encapsulation Mechanism</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>497</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>### JEP 498: Warn upon Use of Memory-Access Methods in sun.misc.Unsafe</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>499</v>
       </c>
@@ -1168,12 +1168,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F25" xr:uid="{3052CF8C-A168-7D4A-AD88-5F8C700EAEB4}">
-    <filterColumn colId="5">
+    <filterColumn colId="3">
       <filters>
-        <filter val="Major"/>
-        <filter val="Minor"/>
-        <filter val="Name changes only"/>
-        <filter val="None"/>
+        <filter val="Security Libs"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Start writing the article on Java 25
</commit_message>
<xml_diff>
--- a/_drafts/jep-overview.xlsx
+++ b/_drafts/jep-overview.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanno/Code/websites/hanno.codes/_drafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68EC1E7-89C4-E949-ADDC-A331C209AB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F22E639-BB62-324E-ABFB-4687311F3E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{D428FD44-A7BE-744F-BBBE-F876344939DC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{D428FD44-A7BE-744F-BBBE-F876344939DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="75">
   <si>
     <t>Status</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Minor</t>
   </si>
   <si>
-    <t>Changes since Java 23</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -210,6 +207,63 @@
   </si>
   <si>
     <t>Streams</t>
+  </si>
+  <si>
+    <t>PEM Encodings of Cryptographic Objects</t>
+  </si>
+  <si>
+    <t>Stable Values</t>
+  </si>
+  <si>
+    <t>Remove the 32-bit x86 Port</t>
+  </si>
+  <si>
+    <t>Fifth Preview</t>
+  </si>
+  <si>
+    <t>Primitive Types in Patterns, instanceof, and switch</t>
+  </si>
+  <si>
+    <t>Tenth Incubator</t>
+  </si>
+  <si>
+    <t>JFR CPU-Time Profiling</t>
+  </si>
+  <si>
+    <t>Compact Source Files and Instance Main Methods</t>
+  </si>
+  <si>
+    <t>Ahead-of-Time Command-Line Ergonomics</t>
+  </si>
+  <si>
+    <t>Ahead-of-Time Method Profiling</t>
+  </si>
+  <si>
+    <t>JFR Cooperative Sampling</t>
+  </si>
+  <si>
+    <t>JFR Method Timing &amp; Tracing</t>
+  </si>
+  <si>
+    <t>New API for constants</t>
+  </si>
+  <si>
+    <t>Removal</t>
+  </si>
+  <si>
+    <t>Changes since Java 24</t>
+  </si>
+  <si>
+    <t>HotSpot / JFR</t>
+  </si>
+  <si>
+    <t>Profiling</t>
+  </si>
+  <si>
+    <t>Stability and performance improvements</t>
+  </si>
+  <si>
+    <t>Java version</t>
   </si>
 </sst>
 </file>
@@ -252,10 +306,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -593,584 +650,1110 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3052CF8C-A168-7D4A-AD88-5F8C700EAEB4}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>24</v>
+      </c>
+      <c r="B2">
         <v>404</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="str">
-        <f>"### JEP "&amp;A2&amp;": "&amp;B2&amp;IF(C2&lt;&gt;""," ("&amp;C2&amp;")","")</f>
+      <c r="G2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="str">
+        <f>"### JEP "&amp;B2&amp;": "&amp;C2&amp;IF(D2&lt;&gt;""," ("&amp;D2&amp;")","")</f>
         <v>### JEP 404: Generational Shenandoah (Experimental)</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>24</v>
+      </c>
+      <c r="B3">
         <v>450</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G25" si="0">"### JEP "&amp;A3&amp;": "&amp;B3&amp;IF(C3&lt;&gt;""," ("&amp;C3&amp;")","")</f>
+      <c r="G3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H43" si="0">"### JEP "&amp;B3&amp;": "&amp;C3&amp;IF(D3&lt;&gt;""," ("&amp;D3&amp;")","")</f>
         <v>### JEP 450: Compact Object Headers (Experimental)</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4">
         <v>472</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 472: Prepare to Restrict the Use of JNI</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>24</v>
+      </c>
+      <c r="B5">
         <v>475</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" t="str">
+      <c r="G5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 475: Late Barrier Expansion for G1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6">
         <v>478</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" t="s">
-        <v>51</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" t="str">
+        <v>50</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 478: Key Derivation Function API (Preview)</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>24</v>
+      </c>
+      <c r="B7">
         <v>479</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>41</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 479: Remove the Windows 32-bit x86 Port</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>24</v>
+      </c>
+      <c r="B8">
         <v>483</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" t="str">
+      <c r="G8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 483: Ahead-of-Time Class Loading &amp; Linking</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>24</v>
+      </c>
+      <c r="B9">
         <v>484</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 484: Class-File API</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
         <v>485</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
-        <v>56</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" t="str">
+        <v>55</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 485: Stream Gatherers</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>24</v>
+      </c>
+      <c r="B11">
         <v>486</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>41</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G11" t="str">
+      <c r="G11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 486: Permanently Disable the Security Manager</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>24</v>
+      </c>
+      <c r="B12">
         <v>487</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
       <c r="F12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 487: Scoped Values (Fourth Preview)</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13">
         <v>488</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E13" t="s">
-        <v>54</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" t="str">
+        <v>53</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 488: Primitive Types in Patterns, instanceof and switch (Second Preview)</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>24</v>
+      </c>
+      <c r="B14">
         <v>489</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" t="str">
+      <c r="G14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 489: Vector API (Ninth Incubator)</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15">
         <v>490</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>41</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G15" t="str">
+      <c r="G15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 490: ZGC: Remove the Non-Generational Mode</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16">
         <v>491</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" t="str">
+        <v>48</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 491: Synchronize Virtual Threads Without Pinning</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17">
         <v>492</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G17" t="str">
+      <c r="G17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 492: Flexible Constructor Bodies (Third Preview)</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18">
         <v>493</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 493: Linking Run-Time Images Without JMODs</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>494</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v>### JEP 493: Linking Run-Time Images Without JMODs</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>494</v>
-      </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="G19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 494: Module Import Declarations (Second Preview)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>495</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="0"/>
-        <v>### JEP 494: Module Import Declarations (Second Preview)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>495</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
       <c r="F20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 495: Simple Source Files and Instance Main Methods (Fourth Preview)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>496</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v>### JEP 495: Simple Source Files and Instance Main Methods (Fourth Preview)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>496</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="G21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 496: Quantum-Resistant Module-Lattice-Based Key Encapsulation Mechanism</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>497</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" si="0"/>
-        <v>### JEP 496: Quantum-Resistant Module-Lattice-Based Key Encapsulation Mechanism</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>497</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" t="s">
-        <v>51</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" t="str">
+        <v>50</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 497: Quantum-Resistant Module-Lattice-Based Digital Signature Algorithm</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23">
         <v>498</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E23" t="s">
-        <v>41</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G23" t="str">
+      <c r="G23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 498: Warn upon Use of Memory-Access Methods in sun.misc.Unsafe</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
         <v>499</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E24" t="s">
-        <v>55</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" t="str">
+        <v>54</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 499: Structured Concurrency (Fourth Preview)</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
         <v>501</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E25" t="s">
-        <v>41</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G25" t="str">
+      <c r="G25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" t="str">
         <f t="shared" si="0"/>
         <v>### JEP 501: Deprecate the 32-bit x86 Port for Removal</v>
       </c>
     </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>470</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 470: PEM Encodings of Cryptographic Objects (Preview)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>502</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 502: Stable Values (Preview)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>503</v>
+      </c>
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 503: Remove the 32-bit x86 Port</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>505</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 505: Structured Concurrency (Fifth Preview)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>506</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 506: Scoped Values</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <v>507</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 507: Primitive Types in Patterns, instanceof, and switch (Third Preview)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>508</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 508: Vector API (Tenth Incubator)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33">
+        <v>509</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" t="str">
+        <f>"### JEP "&amp;B33&amp;": "&amp;C33&amp;IF(D33&lt;&gt;""," ("&amp;D33&amp;")","")</f>
+        <v>### JEP 509: JFR CPU-Time Profiling (Experimental)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>510</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 510: Key Derivation Function API</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35">
+        <v>511</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 511: Module Import Declarations</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>512</v>
+      </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 512: Compact Source Files and Instance Main Methods</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>25</v>
+      </c>
+      <c r="B37">
+        <v>513</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 513: Flexible Constructor Bodies</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>25</v>
+      </c>
+      <c r="B38">
+        <v>514</v>
+      </c>
+      <c r="C38" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H38" t="str">
+        <f>"### JEP "&amp;B38&amp;": "&amp;C38&amp;IF(D38&lt;&gt;""," ("&amp;D38&amp;")","")</f>
+        <v>### JEP 514: Ahead-of-Time Command-Line Ergonomics</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>515</v>
+      </c>
+      <c r="C39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 515: Ahead-of-Time Method Profiling</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>25</v>
+      </c>
+      <c r="B40">
+        <v>518</v>
+      </c>
+      <c r="C40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 518: JFR Cooperative Sampling</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>25</v>
+      </c>
+      <c r="B41">
+        <v>519</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 519: Compact Object Headers</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>25</v>
+      </c>
+      <c r="B42">
+        <v>520</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 520: JFR Method Timing &amp; Tracing</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43">
+        <v>521</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="0"/>
+        <v>### JEP 521: Generational Shenandoah</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F25" xr:uid="{3052CF8C-A168-7D4A-AD88-5F8C700EAEB4}">
-    <filterColumn colId="3">
+  <autoFilter ref="A1:G43" xr:uid="{3052CF8C-A168-7D4A-AD88-5F8C700EAEB4}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Security Libs"/>
+        <filter val="25"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Add article on Java 25
</commit_message>
<xml_diff>
--- a/_drafts/jep-overview.xlsx
+++ b/_drafts/jep-overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanno/Code/websites/hanno.codes/_drafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F22E639-BB62-324E-ABFB-4687311F3E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172BF6F0-7D86-A642-A3C6-B3304148649C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{D428FD44-A7BE-744F-BBBE-F876344939DC}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="21580" xr2:uid="{D428FD44-A7BE-744F-BBBE-F876344939DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -245,9 +245,6 @@
     <t>JFR Method Timing &amp; Tracing</t>
   </si>
   <si>
-    <t>New API for constants</t>
-  </si>
-  <si>
     <t>Removal</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>Java version</t>
+  </si>
+  <si>
+    <t>New API</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="B1" sqref="B1:G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,13 +663,13 @@
     <col min="3" max="3" width="40.5" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -687,7 +687,7 @@
         <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>51</v>
@@ -1343,7 +1343,7 @@
         <v>38</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>46</v>
@@ -1370,7 +1370,7 @@
         <v>41</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -1472,7 +1472,7 @@
         <v>15</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>44</v>
@@ -1496,10 +1496,10 @@
         <v>6</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>46</v>
@@ -1595,7 +1595,7 @@
         <v>21</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>45</v>
@@ -1664,10 +1664,10 @@
         <v>66</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>46</v>
@@ -1712,10 +1712,10 @@
         <v>67</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>46</v>
@@ -1742,7 +1742,7 @@
         <v>42</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>

</xml_diff>